<commit_message>
Atualização GitIgnore e Inclusão do pyprojetct
</commit_message>
<xml_diff>
--- a/eventos.xlsx
+++ b/eventos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Analise_Dados\Projetos\auto-scheduler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3767DE88-88FB-4E4F-9452-AD252A77DBE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FA450F6-D755-432B-AB82-00F0C1ADA98E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Data</t>
   </si>
@@ -31,49 +31,7 @@
     <t>Evento</t>
   </si>
   <si>
-    <t>07:00</t>
-  </si>
-  <si>
-    <t>01/08/2024</t>
-  </si>
-  <si>
-    <t>CONSULTA ELEIRO JOAO PEDRO ELETRO</t>
-  </si>
-  <si>
-    <t>CONSULTA ELETRO AMANDA ELETRO</t>
-  </si>
-  <si>
-    <t>18/07/2024</t>
-  </si>
-  <si>
-    <t>CONSULTA ELETRO JOAO PEDRO ELETRO</t>
-  </si>
-  <si>
-    <t>17/07/2024</t>
-  </si>
-  <si>
-    <t>15/07/2024</t>
-  </si>
-  <si>
-    <t>12/07/2024</t>
-  </si>
-  <si>
-    <t>10/07/2024</t>
-  </si>
-  <si>
-    <t>08/07/2024</t>
-  </si>
-  <si>
-    <t>04/07/2024</t>
-  </si>
-  <si>
-    <t>02/07/2024</t>
-  </si>
-  <si>
-    <t>27/06/2024</t>
-  </si>
-  <si>
-    <t>TESTE AGENDAMENTO PYTHON</t>
+    <t>Python é melhor que Power Automate e qualquer outra ferraemnte de automação, com o maker!!! 😎</t>
   </si>
 </sst>
 </file>
@@ -464,18 +422,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="94.28515625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -490,135 +448,14 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="8" t="s">
+      <c r="A2" s="5">
+        <v>45501</v>
+      </c>
+      <c r="B2" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
-        <v>45492</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="5">
-        <v>45471</v>
-      </c>
-      <c r="B13" s="8">
-        <v>0.375</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>